<commit_message>
zero out BLP for LCFS work
</commit_message>
<xml_diff>
--- a/InputData/trans/BLP/BAU LCFS Perc.xlsx
+++ b/InputData/trans/BLP/BAU LCFS Perc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_Artelys/trans/BLP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\BLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4B205CC6-9ACA-42EA-B56F-0DEE60B3EB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E2F988-486F-4083-8DE4-5D6F49F737B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB75831-616B-4625-AFBF-0138649A39BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{47C8BA48-D4C7-4BCF-988F-BE27F302F0CE}"/>
+    <workbookView xWindow="4545" yWindow="1875" windowWidth="23910" windowHeight="15135" activeTab="2" xr2:uid="{47C8BA48-D4C7-4BCF-988F-BE27F302F0CE}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -262,7 +262,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -399,9 +398,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -439,7 +438,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -545,7 +544,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -687,7 +686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,22 +700,22 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.90625" style="2"/>
-    <col min="3" max="3" width="24.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.90625" style="2"/>
+    <col min="1" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -727,7 +726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="5" t="s">
         <v>18</v>
@@ -736,76 +735,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
@@ -823,21 +822,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4F4E70-1F68-4EEB-960E-6986EB7EB31E}">
   <dimension ref="A2:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.90625" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -845,7 +844,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -854,7 +853,7 @@
         <v>0.14233576642335766</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -863,7 +862,7 @@
         <v>0.1796875</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -871,7 +870,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -879,7 +878,7 @@
         <v>0.21199999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -887,7 +886,7 @@
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -895,7 +894,7 @@
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -903,7 +902,7 @@
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -911,7 +910,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
@@ -919,12 +918,12 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -932,7 +931,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>0.10199999999999999</v>
       </c>
@@ -955,16 +954,16 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="14">
         <v>2020</v>
@@ -1060,133 +1059,102 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="14">
-        <f>'Raw-data'!B19</f>
-        <v>0.10199999999999999</v>
+        <v>0</v>
       </c>
       <c r="C2" s="14">
-        <f>($L$2-$B$2)/($L$1-$B$1)*(C1-$B$1)+$B$2</f>
-        <v>0.10603357664233576</v>
+        <v>0</v>
       </c>
       <c r="D2" s="14">
-        <f t="shared" ref="D2:K2" si="0">($L$2-$B$2)/($L$1-$B$1)*(D1-$B$1)+$B$2</f>
-        <v>0.11006715328467152</v>
+        <v>0</v>
       </c>
       <c r="E2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.11410072992700729</v>
+        <v>0</v>
       </c>
       <c r="F2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.11813430656934307</v>
+        <v>0</v>
       </c>
       <c r="G2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.12216788321167882</v>
+        <v>0</v>
       </c>
       <c r="H2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.1262014598540146</v>
+        <v>0</v>
       </c>
       <c r="I2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.13023503649635038</v>
+        <v>0</v>
       </c>
       <c r="J2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.13426861313868613</v>
+        <v>0</v>
       </c>
       <c r="K2" s="14">
-        <f t="shared" si="0"/>
-        <v>0.13830218978102188</v>
+        <v>0</v>
       </c>
       <c r="L2" s="14">
-        <f>'Raw-data'!B4</f>
-        <v>0.14233576642335766</v>
-      </c>
-      <c r="M2" s="18">
-        <f>TREND($B$2:$L$2,$B$1:$L$1,M1)</f>
-        <v>0.14636934306569316</v>
-      </c>
-      <c r="N2" s="18">
-        <f t="shared" ref="N2:V2" si="1">TREND($B$2:$L$2,$B$1:$L$1,N1)</f>
-        <v>0.15040291970803032</v>
-      </c>
-      <c r="O2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.15443649635036572</v>
-      </c>
-      <c r="P2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.15847007299270111</v>
-      </c>
-      <c r="Q2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.1625036496350365</v>
-      </c>
-      <c r="R2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.16653722627737189</v>
-      </c>
-      <c r="S2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.17057080291970905</v>
-      </c>
-      <c r="T2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.17460437956204444</v>
-      </c>
-      <c r="U2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.17863795620437983</v>
-      </c>
-      <c r="V2" s="18">
-        <f t="shared" si="1"/>
-        <v>0.18267153284671522</v>
-      </c>
-      <c r="W2" s="18">
-        <f>TREND($B$2:$L$2,$B$1:$L$1,W1)</f>
-        <v>0.18670510948905239</v>
-      </c>
-      <c r="X2" s="18">
-        <f t="shared" ref="X2" si="2">TREND($B$2:$L$2,$B$1:$L$1,X1)</f>
-        <v>0.19073868613138778</v>
-      </c>
-      <c r="Y2" s="18">
-        <f t="shared" ref="Y2" si="3">TREND($B$2:$L$2,$B$1:$L$1,Y1)</f>
-        <v>0.19477226277372317</v>
-      </c>
-      <c r="Z2" s="18">
-        <f t="shared" ref="Z2" si="4">TREND($B$2:$L$2,$B$1:$L$1,Z1)</f>
-        <v>0.19880583941605856</v>
-      </c>
-      <c r="AA2" s="18">
-        <f t="shared" ref="AA2" si="5">TREND($B$2:$L$2,$B$1:$L$1,AA1)</f>
-        <v>0.20283941605839395</v>
-      </c>
-      <c r="AB2" s="18">
-        <f t="shared" ref="AB2" si="6">TREND($B$2:$L$2,$B$1:$L$1,AB1)</f>
-        <v>0.20687299270073112</v>
-      </c>
-      <c r="AC2" s="18">
-        <f t="shared" ref="AC2" si="7">TREND($B$2:$L$2,$B$1:$L$1,AC1)</f>
-        <v>0.21090656934306651</v>
-      </c>
-      <c r="AD2" s="18">
-        <f t="shared" ref="AD2" si="8">TREND($B$2:$L$2,$B$1:$L$1,AD1)</f>
-        <v>0.2149401459854019</v>
-      </c>
-      <c r="AE2" s="18">
-        <f t="shared" ref="AE2" si="9">TREND($B$2:$L$2,$B$1:$L$1,AE1)</f>
-        <v>0.21897372262773729</v>
-      </c>
-      <c r="AF2" s="18">
-        <f t="shared" ref="AF2" si="10">TREND($B$2:$L$2,$B$1:$L$1,AF1)</f>
-        <v>0.22300729927007268</v>
+        <v>0</v>
+      </c>
+      <c r="M2" s="14">
+        <v>0</v>
+      </c>
+      <c r="N2" s="14">
+        <v>0</v>
+      </c>
+      <c r="O2" s="14">
+        <v>0</v>
+      </c>
+      <c r="P2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+      <c r="R2" s="14">
+        <v>0</v>
+      </c>
+      <c r="S2" s="14">
+        <v>0</v>
+      </c>
+      <c r="T2" s="14">
+        <v>0</v>
+      </c>
+      <c r="U2" s="14">
+        <v>0</v>
+      </c>
+      <c r="V2" s="14">
+        <v>0</v>
+      </c>
+      <c r="W2" s="14">
+        <v>0</v>
+      </c>
+      <c r="X2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1206,6 +1174,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -1428,15 +1405,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{880F3CA1-459A-43A6-9BDC-271E9A326C86}">
   <ds:schemaRefs>
@@ -1449,6 +1417,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{378D7905-FE87-4243-B092-6DB7BD4C286E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{450CD3D1-EE04-4F21-B653-6CA85E520643}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1465,12 +1441,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{378D7905-FE87-4243-B092-6DB7BD4C286E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>